<commit_message>
update temp DEQM R4 view
</commit_message>
<xml_diff>
--- a/docs/datax-measurereport-deqm.xlsx
+++ b/docs/datax-measurereport-deqm.xlsx
@@ -147,7 +147,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.div.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}mrp-2:Stratifiers SHALL be either a single criteria or a set of criteria components {group.stratifier.stratum.all(value.exists() xor component.exists())}mrp-1:Measure Reports used for data collection SHALL NOT communicate group and score information {(type != 'data-collection') or group.exists().not()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}mrp-1:Measure Reports used for data collection SHALL NOT communicate group and score information {(type != 'data-collection') or group.exists().not()}mrp-2:Stratifiers SHALL be either a single criteria or a set of criteria components {group.stratifier.stratum.all(value.exists() xor component.exists())}</t>
   </si>
   <si>
     <t>Entity. Role, or Act</t>
@@ -162,7 +162,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -194,6 +194,10 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+</t>
+  </si>
+  <si>
     <t>MeasureReport.implicitRules</t>
   </si>
   <si>
@@ -316,6 +320,10 @@
     <t>DomainResource.extension</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
     <t>MeasureReport.modifierExtension</t>
   </si>
   <si>
@@ -393,7 +401,7 @@
     <t>The type of the measure report.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/measure-report-type|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/measure-report-type|4.0.1</t>
   </si>
   <si>
     <t xml:space="preserve">mrp-1
@@ -487,15 +495,11 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">deqm-1:Date precision SHALL  be at least to day ( YYYY-MM-DD ) {start.matches('^([0-9]{4})(-)(1[0-2]|0[1-9])-(3[01]|0[1-9]|[12][0-9])') and end.matches('^([0-9]{4})(-)(1[0-2]|0[1-9])-(3[01]|0[1-9]|[12][0-9])')}
-</t>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+deqm-1:Date precision SHALL  be at least to day ( YYYY-MM-DD ) {start.matches('^([0-9]{4})(-)(1[0-2]|0[1-9])-(3[01]|0[1-9]|[12][0-9])') and end.matches('^([0-9]{4})(-)(1[0-2]|0[1-9])-(3[01]|0[1-9]|[12][0-9])')}</t>
   </si>
   <si>
     <t>MeasureReport.period.id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
   </si>
   <si>
     <t>Unique id for inter-element referencing</t>
@@ -591,7 +595,7 @@
     <t>Observation values that indicate what change in a measurement value or score is indicative of an improvement in the measured item or scored issue.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/measure-improvement-notation|4.0.0</t>
+    <t>http://hl7.org/fhir/ValueSet/measure-improvement-notation|4.0.1</t>
   </si>
   <si>
     <t>MeasureReport.group</t>
@@ -605,10 +609,6 @@
   </si>
   <si>
     <t>The results of the calculation, one for each population group in the measure.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-</t>
   </si>
   <si>
     <t>MeasureReport.group.id</t>
@@ -1472,7 +1472,7 @@
         <v>38</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>38</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1506,16 +1506,16 @@
         <v>47</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -1565,7 +1565,7 @@
         <v>38</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>39</v>
@@ -1577,7 +1577,7 @@
         <v>38</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ5" t="s" s="2">
         <v>38</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -1611,16 +1611,16 @@
         <v>38</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -1646,13 +1646,13 @@
         <v>38</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>38</v>
@@ -1670,7 +1670,7 @@
         <v>38</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>39</v>
@@ -1682,7 +1682,7 @@
         <v>38</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>38</v>
@@ -1693,11 +1693,11 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
@@ -1716,16 +1716,16 @@
         <v>38</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -1775,7 +1775,7 @@
         <v>38</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>39</v>
@@ -1787,22 +1787,22 @@
         <v>38</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -1821,16 +1821,16 @@
         <v>38</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -1880,7 +1880,7 @@
         <v>38</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>39</v>
@@ -1898,16 +1898,16 @@
         <v>38</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -1926,16 +1926,16 @@
         <v>38</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -1985,7 +1985,7 @@
         <v>38</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>39</v>
@@ -1997,22 +1997,22 @@
         <v>38</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -2031,19 +2031,19 @@
         <v>38</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="O10" t="s" s="2">
         <v>38</v>
@@ -2092,7 +2092,7 @@
         <v>38</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>39</v>
@@ -2104,18 +2104,18 @@
         <v>38</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -2138,19 +2138,19 @@
         <v>47</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="O11" t="s" s="2">
         <v>38</v>
@@ -2199,7 +2199,7 @@
         <v>38</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>39</v>
@@ -2211,10 +2211,10 @@
         <v>38</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AK11" t="s" s="2">
         <v>38</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2245,16 +2245,16 @@
         <v>47</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -2280,11 +2280,11 @@
         <v>38</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" t="s" s="2">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>38</v>
@@ -2302,7 +2302,7 @@
         <v>38</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>46</v>
@@ -2314,10 +2314,10 @@
         <v>38</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>38</v>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2348,16 +2348,16 @@
         <v>47</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -2365,7 +2365,7 @@
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" t="s" s="2">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="R13" t="s" s="2">
         <v>38</v>
@@ -2383,13 +2383,13 @@
         <v>38</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>38</v>
@@ -2407,7 +2407,7 @@
         <v>38</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>46</v>
@@ -2416,13 +2416,13 @@
         <v>46</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>38</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2453,17 +2453,17 @@
         <v>47</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="O14" t="s" s="2">
         <v>38</v>
@@ -2512,7 +2512,7 @@
         <v>38</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>46</v>
@@ -2524,10 +2524,10 @@
         <v>38</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>38</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2558,13 +2558,13 @@
         <v>47</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2615,7 +2615,7 @@
         <v>38</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>39</v>
@@ -2627,10 +2627,10 @@
         <v>38</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>38</v>
@@ -2638,7 +2638,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2661,13 +2661,13 @@
         <v>47</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2718,7 +2718,7 @@
         <v>38</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>39</v>
@@ -2730,10 +2730,10 @@
         <v>38</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>38</v>
@@ -2741,7 +2741,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2764,13 +2764,13 @@
         <v>47</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2821,7 +2821,7 @@
         <v>38</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>39</v>
@@ -2833,10 +2833,10 @@
         <v>38</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>38</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2867,13 +2867,13 @@
         <v>47</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2924,7 +2924,7 @@
         <v>38</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>46</v>
@@ -2933,10 +2933,10 @@
         <v>46</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>38</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -2970,13 +2970,13 @@
         <v>38</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3027,7 +3027,7 @@
         <v>38</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>39</v>
@@ -3045,16 +3045,16 @@
         <v>38</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3073,16 +3073,16 @@
         <v>38</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3120,19 +3120,19 @@
         <v>38</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AB20" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AC20" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AD20" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
@@ -3144,18 +3144,18 @@
         <v>38</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3178,16 +3178,16 @@
         <v>47</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3237,7 +3237,7 @@
         <v>38</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>39</v>
@@ -3246,21 +3246,21 @@
         <v>46</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3283,23 +3283,23 @@
         <v>47</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>38</v>
       </c>
       <c r="P22" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Q22" t="s" s="2">
         <v>38</v>
@@ -3344,7 +3344,7 @@
         <v>38</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>39</v>
@@ -3353,21 +3353,21 @@
         <v>46</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3390,16 +3390,16 @@
         <v>47</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -3425,13 +3425,13 @@
         <v>38</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>38</v>
@@ -3449,7 +3449,7 @@
         <v>38</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
@@ -3461,7 +3461,7 @@
         <v>38</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>38</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3495,13 +3495,13 @@
         <v>38</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3552,7 +3552,7 @@
         <v>38</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>39</v>
@@ -3561,10 +3561,10 @@
         <v>40</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>38</v>
@@ -3598,13 +3598,13 @@
         <v>38</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -3655,7 +3655,7 @@
         <v>38</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
@@ -3673,7 +3673,7 @@
         <v>38</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" hidden="true">
@@ -3682,7 +3682,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -3701,16 +3701,16 @@
         <v>38</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
@@ -3760,7 +3760,7 @@
         <v>38</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>39</v>
@@ -3772,13 +3772,13 @@
         <v>38</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" hidden="true">
@@ -3806,7 +3806,7 @@
         <v>47</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K27" t="s" s="2">
         <v>193</v>
@@ -3815,10 +3815,10 @@
         <v>194</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>38</v>
@@ -3879,13 +3879,13 @@
         <v>38</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" hidden="true">
@@ -3913,7 +3913,7 @@
         <v>47</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K28" t="s" s="2">
         <v>197</v>
@@ -3982,7 +3982,7 @@
         <v>38</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>38</v>
@@ -4016,7 +4016,7 @@
         <v>38</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K29" t="s" s="2">
         <v>200</v>
@@ -4085,7 +4085,7 @@
         <v>38</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>38</v>
@@ -4119,13 +4119,13 @@
         <v>38</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4176,7 +4176,7 @@
         <v>38</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
@@ -4194,7 +4194,7 @@
         <v>38</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" hidden="true">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
@@ -4222,16 +4222,16 @@
         <v>38</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4281,7 +4281,7 @@
         <v>38</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>39</v>
@@ -4293,13 +4293,13 @@
         <v>38</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" hidden="true">
@@ -4327,7 +4327,7 @@
         <v>47</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K32" t="s" s="2">
         <v>193</v>
@@ -4336,10 +4336,10 @@
         <v>194</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>38</v>
@@ -4400,13 +4400,13 @@
         <v>38</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" hidden="true">
@@ -4434,7 +4434,7 @@
         <v>47</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K33" t="s" s="2">
         <v>206</v>
@@ -4503,7 +4503,7 @@
         <v>38</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>38</v>
@@ -4606,7 +4606,7 @@
         <v>38</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>38</v>
@@ -4709,7 +4709,7 @@
         <v>38</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>38</v>
@@ -4812,7 +4812,7 @@
         <v>38</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>38</v>
@@ -4846,7 +4846,7 @@
         <v>38</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K37" t="s" s="2">
         <v>224</v>
@@ -4915,7 +4915,7 @@
         <v>38</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>38</v>
@@ -4949,13 +4949,13 @@
         <v>38</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5006,7 +5006,7 @@
         <v>38</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>39</v>
@@ -5024,7 +5024,7 @@
         <v>38</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" hidden="true">
@@ -5033,7 +5033,7 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5052,16 +5052,16 @@
         <v>38</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -5111,7 +5111,7 @@
         <v>38</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>39</v>
@@ -5123,13 +5123,13 @@
         <v>38</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" hidden="true">
@@ -5157,7 +5157,7 @@
         <v>47</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K40" t="s" s="2">
         <v>193</v>
@@ -5166,10 +5166,10 @@
         <v>194</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>38</v>
@@ -5230,13 +5230,13 @@
         <v>38</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" hidden="true">
@@ -5264,7 +5264,7 @@
         <v>38</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K41" t="s" s="2">
         <v>230</v>
@@ -5333,7 +5333,7 @@
         <v>38</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ41" t="s" s="2">
         <v>38</v>
@@ -5367,7 +5367,7 @@
         <v>38</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K42" t="s" s="2">
         <v>233</v>
@@ -5436,7 +5436,7 @@
         <v>38</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>38</v>
@@ -5470,13 +5470,13 @@
         <v>38</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -5527,7 +5527,7 @@
         <v>38</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>39</v>
@@ -5545,7 +5545,7 @@
         <v>38</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" hidden="true">
@@ -5554,7 +5554,7 @@
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
@@ -5573,16 +5573,16 @@
         <v>38</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -5632,7 +5632,7 @@
         <v>38</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>39</v>
@@ -5644,13 +5644,13 @@
         <v>38</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" hidden="true">
@@ -5678,7 +5678,7 @@
         <v>47</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K45" t="s" s="2">
         <v>193</v>
@@ -5687,10 +5687,10 @@
         <v>194</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>38</v>
@@ -5751,13 +5751,13 @@
         <v>38</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" hidden="true">
@@ -5785,7 +5785,7 @@
         <v>38</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K46" t="s" s="2">
         <v>239</v>
@@ -5854,7 +5854,7 @@
         <v>38</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>38</v>
@@ -5888,7 +5888,7 @@
         <v>38</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K47" t="s" s="2">
         <v>242</v>
@@ -5957,7 +5957,7 @@
         <v>38</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>38</v>
@@ -5991,13 +5991,13 @@
         <v>38</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6048,7 +6048,7 @@
         <v>38</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>39</v>
@@ -6066,7 +6066,7 @@
         <v>38</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" hidden="true">
@@ -6075,7 +6075,7 @@
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -6094,16 +6094,16 @@
         <v>38</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -6153,7 +6153,7 @@
         <v>38</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>39</v>
@@ -6165,13 +6165,13 @@
         <v>38</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" hidden="true">
@@ -6199,7 +6199,7 @@
         <v>47</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K50" t="s" s="2">
         <v>193</v>
@@ -6208,10 +6208,10 @@
         <v>194</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>38</v>
@@ -6272,13 +6272,13 @@
         <v>38</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" hidden="true">
@@ -6306,7 +6306,7 @@
         <v>38</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K51" t="s" s="2">
         <v>248</v>
@@ -6375,7 +6375,7 @@
         <v>38</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>38</v>
@@ -6409,7 +6409,7 @@
         <v>38</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K52" t="s" s="2">
         <v>251</v>
@@ -6478,7 +6478,7 @@
         <v>38</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>38</v>
@@ -6512,7 +6512,7 @@
         <v>38</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K53" t="s" s="2">
         <v>254</v>
@@ -6581,7 +6581,7 @@
         <v>38</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="AJ53" t="s" s="2">
         <v>38</v>
@@ -6615,13 +6615,13 @@
         <v>38</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -6672,7 +6672,7 @@
         <v>38</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>39</v>
@@ -6690,7 +6690,7 @@
         <v>38</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" hidden="true">
@@ -6699,7 +6699,7 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -6718,16 +6718,16 @@
         <v>38</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -6777,7 +6777,7 @@
         <v>38</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>39</v>
@@ -6789,13 +6789,13 @@
         <v>38</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" hidden="true">
@@ -6823,7 +6823,7 @@
         <v>47</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K56" t="s" s="2">
         <v>193</v>
@@ -6832,10 +6832,10 @@
         <v>194</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>38</v>
@@ -6896,13 +6896,13 @@
         <v>38</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" hidden="true">
@@ -6930,7 +6930,7 @@
         <v>38</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K57" t="s" s="2">
         <v>206</v>
@@ -6999,7 +6999,7 @@
         <v>38</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ57" t="s" s="2">
         <v>38</v>
@@ -7102,7 +7102,7 @@
         <v>38</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>38</v>
@@ -7205,7 +7205,7 @@
         <v>38</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ59" t="s" s="2">
         <v>38</v>
@@ -7308,7 +7308,7 @@
         <v>38</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>38</v>
@@ -7411,7 +7411,7 @@
         <v>38</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>38</v>

</xml_diff>